<commit_message>
PDF CM optimizacion de codigo y pruebas de las diferentes logisticas (correciones)
PDF CM optimizacion de codigo y pruebas de las diferentes logisticas (correciones)
</commit_message>
<xml_diff>
--- a/public/downloads/Base.xlsx
+++ b/public/downloads/Base.xlsx
@@ -87,9 +87,6 @@
     <t>Unidad</t>
   </si>
   <si>
-    <t>Tipo Unidad</t>
-  </si>
-  <si>
     <t>NOTAS:</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>N°2: Estatus colocar Terminado o Cancelado, en caso de no colocar nada, por default el viaje tendra estatus Terminado</t>
+  </si>
+  <si>
+    <t>Placa (Remolque o Tonel)</t>
   </si>
 </sst>
 </file>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +543,7 @@
     <col min="25" max="25" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" s="2" customFormat="1" ht="35.25" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:25" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -551,7 +551,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>0</v>
@@ -614,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="Y3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
     </row>
     <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>